<commit_message>
Project 1 Code complete, rough draft done
</commit_message>
<xml_diff>
--- a/Project Reflections/P1 Reflection/SubmissionResults.xlsx
+++ b/Project Reflections/P1 Reflection/SubmissionResults.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="6June" sheetId="1" r:id="rId1"/>
+    <sheet name="8June" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Correct</t>
   </si>
@@ -475,11 +476,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246271088"/>
-        <c:axId val="246271480"/>
+        <c:axId val="221395776"/>
+        <c:axId val="392551832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246271088"/>
+        <c:axId val="221395776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246271480"/>
+        <c:crossAx val="392551832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -530,7 +531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246271480"/>
+        <c:axId val="392551832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +582,583 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246271088"/>
+        <c:crossAx val="221395776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Correct</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Incorrect</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8June'!$B$6:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'8June'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'8June'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Basic Problems B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Challenge Problems B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ravens Problems B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test Problems B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8June'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'8June'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incorrect</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'8June'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Basic Problems B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Challenge Problems B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ravens Problems B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test Problems B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8June'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="397034952"/>
+        <c:axId val="397038480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="397034952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397038480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397038480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397034952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -742,6 +1319,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -1262,6 +1919,1030 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1815,6 +3496,75 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>415290</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>110490</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2120,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,4 +3945,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C5)</f>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>